<commit_message>
minor changes to manual tests
</commit_message>
<xml_diff>
--- a/Relayr_EmployeeMS_APITests_Manual.xlsx
+++ b/Relayr_EmployeeMS_APITests_Manual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madhan/TreeView/relayr/Task2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madhan/TreeView/relayr/Task2/Relayr_EmployeeMS_APITestSuite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6947F5A2-C205-D34B-9137-3AEFE5474043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3273C844-87FF-EB49-ABB3-BD61BC36B3EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="151">
   <si>
     <t>Reference Material</t>
   </si>
@@ -751,12 +751,18 @@
   <si>
     <t>Updated</t>
   </si>
+  <si>
+    <t>Employee Management System or EMS is a service to maintain employee data within relayr</t>
+  </si>
+  <si>
+    <t>All tests needs to executed manually using Postman tool</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -799,14 +805,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -868,6 +866,28 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1047,37 +1067,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1086,7 +1106,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1095,20 +1115,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1128,6 +1144,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1180,6 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
@@ -4908,7 +4931,9 @@
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="24"/>
+      <c r="E3" s="23" t="s">
+        <v>149</v>
+      </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
@@ -5026,7 +5051,9 @@
       <c r="C11" s="12">
         <v>43540</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="23" t="s">
+        <v>150</v>
+      </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -5205,7 +5232,7 @@
     <col min="6" max="6" width="44.1640625" customWidth="1"/>
     <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="56.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="23" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="51" customWidth="1"/>
     <col min="11" max="13" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5350,19 +5377,19 @@
       <c r="A9" s="37">
         <v>1</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="32" t="s">
         <v>56</v>
       </c>
       <c r="E9" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="32" t="s">
         <v>61</v>
       </c>
       <c r="G9" s="15" t="s">
@@ -5375,21 +5402,21 @@
       <c r="J9" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="M9" s="26"/>
+      <c r="M9" s="32"/>
     </row>
     <row r="10" spans="1:13" ht="32">
       <c r="A10" s="37"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="38"/>
-      <c r="F10" s="27"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="15" t="s">
         <v>81</v>
       </c>
@@ -5398,17 +5425,17 @@
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="39"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="26"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="32"/>
     </row>
     <row r="11" spans="1:13" ht="409" customHeight="1">
       <c r="A11" s="37"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="38"/>
-      <c r="F11" s="27"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="15" t="s">
         <v>52</v>
       </c>
@@ -5417,17 +5444,17 @@
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="39"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="26"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="32"/>
     </row>
     <row r="12" spans="1:13" ht="32">
       <c r="A12" s="37"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="38"/>
-      <c r="F12" s="27"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="15" t="s">
         <v>55</v>
       </c>
@@ -5436,24 +5463,24 @@
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="39"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="26"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="32"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
     </row>
     <row r="14" spans="1:13" ht="16">
       <c r="A14" s="40">
@@ -5484,10 +5511,10 @@
       <c r="J14" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="K14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="29" t="s">
         <v>143</v>
       </c>
       <c r="M14" s="34"/>
@@ -5507,8 +5534,8 @@
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="47"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
       <c r="M15" s="35"/>
     </row>
     <row r="16" spans="1:13" ht="112">
@@ -5526,8 +5553,8 @@
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="47"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
       <c r="M16" s="35"/>
     </row>
     <row r="17" spans="1:13" ht="129" customHeight="1">
@@ -5545,8 +5572,8 @@
       </c>
       <c r="I17" s="18"/>
       <c r="J17" s="48"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
       <c r="M17" s="36"/>
     </row>
     <row r="18" spans="1:13">
@@ -5593,10 +5620,10 @@
       <c r="J19" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="31" t="s">
+      <c r="K19" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="L19" s="31" t="s">
+      <c r="L19" s="29" t="s">
         <v>143</v>
       </c>
       <c r="M19" s="34"/>
@@ -5616,8 +5643,8 @@
       </c>
       <c r="I20" s="18"/>
       <c r="J20" s="47"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
       <c r="M20" s="35"/>
     </row>
     <row r="21" spans="1:13" ht="112">
@@ -5635,8 +5662,8 @@
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="47"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
       <c r="M21" s="35"/>
     </row>
     <row r="22" spans="1:13" ht="129" customHeight="1">
@@ -5654,42 +5681,42 @@
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="48"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
       <c r="M22" s="36"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="29"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
     </row>
     <row r="24" spans="1:13" ht="16">
       <c r="A24" s="37">
         <v>4</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="32" t="s">
         <v>66</v>
       </c>
       <c r="E24" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="32" t="s">
         <v>72</v>
       </c>
       <c r="G24" s="15" t="s">
@@ -5702,21 +5729,21 @@
       <c r="J24" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="30" t="s">
+      <c r="K24" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L24" s="30" t="s">
+      <c r="L24" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="M24" s="26"/>
+      <c r="M24" s="32"/>
     </row>
     <row r="25" spans="1:13" ht="32">
       <c r="A25" s="37"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="38"/>
-      <c r="F25" s="27"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="15" t="s">
         <v>81</v>
       </c>
@@ -5725,17 +5752,17 @@
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="39"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="26"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="32"/>
     </row>
     <row r="26" spans="1:13" ht="395" customHeight="1">
       <c r="A26" s="37"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
       <c r="E26" s="38"/>
-      <c r="F26" s="27"/>
+      <c r="F26" s="33"/>
       <c r="G26" s="15" t="s">
         <v>52</v>
       </c>
@@ -5744,17 +5771,17 @@
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="39"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="26"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="32"/>
     </row>
     <row r="27" spans="1:13" ht="32">
       <c r="A27" s="37"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="38"/>
-      <c r="F27" s="27"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="15" t="s">
         <v>55</v>
       </c>
@@ -5763,42 +5790,42 @@
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="39"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="26"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="32"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="29"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="27"/>
     </row>
     <row r="29" spans="1:13" ht="16">
       <c r="A29" s="37">
         <v>5</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="32" t="s">
         <v>98</v>
       </c>
       <c r="E29" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="32" t="s">
         <v>76</v>
       </c>
       <c r="G29" s="15" t="s">
@@ -5811,21 +5838,21 @@
       <c r="J29" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="30" t="s">
+      <c r="K29" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L29" s="30" t="s">
+      <c r="L29" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="M29" s="26"/>
+      <c r="M29" s="32"/>
     </row>
     <row r="30" spans="1:13" ht="32">
       <c r="A30" s="37"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="33"/>
       <c r="G30" s="15" t="s">
         <v>81</v>
       </c>
@@ -5834,17 +5861,17 @@
       </c>
       <c r="I30" s="18"/>
       <c r="J30" s="39"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="26"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="32"/>
     </row>
     <row r="31" spans="1:13" ht="112">
       <c r="A31" s="37"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="27"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="15" t="s">
         <v>52</v>
       </c>
@@ -5853,17 +5880,17 @@
       </c>
       <c r="I31" s="18"/>
       <c r="J31" s="39"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="26"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="32"/>
     </row>
     <row r="32" spans="1:13" ht="32">
       <c r="A32" s="37"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="38"/>
-      <c r="F32" s="27"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="15" t="s">
         <v>55</v>
       </c>
@@ -5872,42 +5899,42 @@
       </c>
       <c r="I32" s="18"/>
       <c r="J32" s="39"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="26"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="29"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="27"/>
     </row>
     <row r="34" spans="1:13" ht="16">
       <c r="A34" s="37">
         <v>6</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="32" t="s">
         <v>99</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="26" t="s">
+      <c r="F34" s="32" t="s">
         <v>118</v>
       </c>
       <c r="G34" s="15" t="s">
@@ -5920,21 +5947,21 @@
       <c r="J34" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K34" s="30" t="s">
+      <c r="K34" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L34" s="30" t="s">
+      <c r="L34" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="M34" s="26"/>
+      <c r="M34" s="32"/>
     </row>
     <row r="35" spans="1:13" ht="32">
       <c r="A35" s="37"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="38"/>
-      <c r="F35" s="27"/>
+      <c r="F35" s="33"/>
       <c r="G35" s="15" t="s">
         <v>81</v>
       </c>
@@ -5943,17 +5970,17 @@
       </c>
       <c r="I35" s="18"/>
       <c r="J35" s="39"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="26"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="32"/>
     </row>
     <row r="36" spans="1:13" ht="144" customHeight="1">
       <c r="A36" s="37"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="38"/>
-      <c r="F36" s="27"/>
+      <c r="F36" s="33"/>
       <c r="G36" s="15" t="s">
         <v>52</v>
       </c>
@@ -5962,17 +5989,17 @@
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="39"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="26"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="32"/>
     </row>
     <row r="37" spans="1:13" ht="32">
       <c r="A37" s="37"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="38"/>
-      <c r="F37" s="27"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="15" t="s">
         <v>55</v>
       </c>
@@ -5981,42 +6008,42 @@
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="39"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="26"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="29"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="27"/>
     </row>
     <row r="39" spans="1:13" ht="16">
       <c r="A39" s="37">
         <v>7</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="32" t="s">
         <v>79</v>
       </c>
       <c r="E39" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="32" t="s">
         <v>88</v>
       </c>
       <c r="G39" s="15" t="s">
@@ -6029,21 +6056,21 @@
       <c r="J39" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K39" s="30" t="s">
+      <c r="K39" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L39" s="30" t="s">
+      <c r="L39" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="M39" s="26"/>
+      <c r="M39" s="32"/>
     </row>
     <row r="40" spans="1:13" ht="32">
       <c r="A40" s="37"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
       <c r="E40" s="38"/>
-      <c r="F40" s="27"/>
+      <c r="F40" s="33"/>
       <c r="G40" s="15" t="s">
         <v>81</v>
       </c>
@@ -6052,17 +6079,17 @@
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="39"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="26"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="32"/>
     </row>
     <row r="41" spans="1:13" ht="32">
       <c r="A41" s="37"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="38"/>
-      <c r="F41" s="27"/>
+      <c r="F41" s="33"/>
       <c r="G41" s="15" t="s">
         <v>83</v>
       </c>
@@ -6071,17 +6098,17 @@
       </c>
       <c r="I41" s="18"/>
       <c r="J41" s="39"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="30"/>
-      <c r="M41" s="26"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="32"/>
     </row>
     <row r="42" spans="1:13" ht="256">
       <c r="A42" s="37"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
       <c r="E42" s="38"/>
-      <c r="F42" s="27"/>
+      <c r="F42" s="33"/>
       <c r="G42" s="15" t="s">
         <v>89</v>
       </c>
@@ -6090,17 +6117,17 @@
       </c>
       <c r="I42" s="18"/>
       <c r="J42" s="39"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="26"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="32"/>
     </row>
     <row r="43" spans="1:13" ht="48">
       <c r="A43" s="37"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
       <c r="E43" s="38"/>
-      <c r="F43" s="27"/>
+      <c r="F43" s="33"/>
       <c r="G43" s="15" t="s">
         <v>92</v>
       </c>
@@ -6109,17 +6136,17 @@
       </c>
       <c r="I43" s="18"/>
       <c r="J43" s="39"/>
-      <c r="K43" s="30"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="26"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="32"/>
     </row>
     <row r="44" spans="1:13" ht="32">
       <c r="A44" s="37"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
       <c r="E44" s="38"/>
-      <c r="F44" s="27"/>
+      <c r="F44" s="33"/>
       <c r="G44" s="15" t="s">
         <v>94</v>
       </c>
@@ -6128,17 +6155,17 @@
       </c>
       <c r="I44" s="18"/>
       <c r="J44" s="39"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="26"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="32"/>
     </row>
     <row r="45" spans="1:13" ht="32">
       <c r="A45" s="37"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
       <c r="E45" s="38"/>
-      <c r="F45" s="27"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="15" t="s">
         <v>95</v>
       </c>
@@ -6147,42 +6174,42 @@
       </c>
       <c r="I45" s="18"/>
       <c r="J45" s="39"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="26"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="32"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="29"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="27"/>
     </row>
     <row r="47" spans="1:13" ht="16">
       <c r="A47" s="37">
         <v>8</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="32" t="s">
         <v>100</v>
       </c>
       <c r="E47" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="F47" s="26" t="s">
+      <c r="F47" s="32" t="s">
         <v>101</v>
       </c>
       <c r="G47" s="15" t="s">
@@ -6195,21 +6222,21 @@
       <c r="J47" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K47" s="30" t="s">
+      <c r="K47" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L47" s="30" t="s">
+      <c r="L47" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="M47" s="26"/>
+      <c r="M47" s="32"/>
     </row>
     <row r="48" spans="1:13" ht="32">
       <c r="A48" s="37"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="38"/>
-      <c r="F48" s="27"/>
+      <c r="F48" s="33"/>
       <c r="G48" s="15" t="s">
         <v>81</v>
       </c>
@@ -6218,17 +6245,17 @@
       </c>
       <c r="I48" s="18"/>
       <c r="J48" s="39"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="26"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="32"/>
     </row>
     <row r="49" spans="1:13" ht="32">
       <c r="A49" s="37"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="38"/>
-      <c r="F49" s="27"/>
+      <c r="F49" s="33"/>
       <c r="G49" s="15" t="s">
         <v>83</v>
       </c>
@@ -6237,17 +6264,17 @@
       </c>
       <c r="I49" s="18"/>
       <c r="J49" s="39"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="26"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="32"/>
     </row>
     <row r="50" spans="1:13" ht="112">
       <c r="A50" s="37"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="38"/>
-      <c r="F50" s="27"/>
+      <c r="F50" s="33"/>
       <c r="G50" s="15" t="s">
         <v>89</v>
       </c>
@@ -6256,17 +6283,17 @@
       </c>
       <c r="I50" s="18"/>
       <c r="J50" s="39"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="30"/>
-      <c r="M50" s="26"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="32"/>
     </row>
     <row r="51" spans="1:13" ht="32">
       <c r="A51" s="37"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="38"/>
-      <c r="F51" s="27"/>
+      <c r="F51" s="33"/>
       <c r="G51" s="15" t="s">
         <v>102</v>
       </c>
@@ -6275,17 +6302,17 @@
       </c>
       <c r="I51" s="18"/>
       <c r="J51" s="39"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="26"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="32"/>
     </row>
     <row r="52" spans="1:13" ht="32">
       <c r="A52" s="37"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="38"/>
-      <c r="F52" s="27"/>
+      <c r="F52" s="33"/>
       <c r="G52" s="15" t="s">
         <v>104</v>
       </c>
@@ -6294,42 +6321,42 @@
       </c>
       <c r="I52" s="18"/>
       <c r="J52" s="39"/>
-      <c r="K52" s="30"/>
-      <c r="L52" s="30"/>
-      <c r="M52" s="26"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="32"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="29"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="27"/>
     </row>
     <row r="54" spans="1:13" ht="16">
       <c r="A54" s="37">
         <v>9</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="26" t="s">
+      <c r="C54" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D54" s="26" t="s">
+      <c r="D54" s="32" t="s">
         <v>107</v>
       </c>
       <c r="E54" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="F54" s="26" t="s">
+      <c r="F54" s="32" t="s">
         <v>112</v>
       </c>
       <c r="G54" s="15" t="s">
@@ -6342,21 +6369,21 @@
       <c r="J54" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K54" s="30" t="s">
+      <c r="K54" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L54" s="30" t="s">
+      <c r="L54" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="M54" s="26"/>
+      <c r="M54" s="32"/>
     </row>
     <row r="55" spans="1:13" ht="32">
       <c r="A55" s="37"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="38"/>
-      <c r="F55" s="27"/>
+      <c r="F55" s="33"/>
       <c r="G55" s="15" t="s">
         <v>81</v>
       </c>
@@ -6365,17 +6392,17 @@
       </c>
       <c r="I55" s="18"/>
       <c r="J55" s="39"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="26"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="32"/>
     </row>
     <row r="56" spans="1:13" ht="32">
       <c r="A56" s="37"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
       <c r="E56" s="38"/>
-      <c r="F56" s="27"/>
+      <c r="F56" s="33"/>
       <c r="G56" s="15" t="s">
         <v>83</v>
       </c>
@@ -6384,17 +6411,17 @@
       </c>
       <c r="I56" s="18"/>
       <c r="J56" s="39"/>
-      <c r="K56" s="30"/>
-      <c r="L56" s="30"/>
-      <c r="M56" s="26"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="32"/>
     </row>
     <row r="57" spans="1:13" ht="240">
       <c r="A57" s="37"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="38"/>
-      <c r="F57" s="27"/>
+      <c r="F57" s="33"/>
       <c r="G57" s="15" t="s">
         <v>89</v>
       </c>
@@ -6403,17 +6430,17 @@
       </c>
       <c r="I57" s="18"/>
       <c r="J57" s="39"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="30"/>
-      <c r="M57" s="26"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="32"/>
     </row>
     <row r="58" spans="1:13" ht="32">
       <c r="A58" s="37"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
       <c r="E58" s="38"/>
-      <c r="F58" s="27"/>
+      <c r="F58" s="33"/>
       <c r="G58" s="15" t="s">
         <v>123</v>
       </c>
@@ -6422,17 +6449,17 @@
       </c>
       <c r="I58" s="18"/>
       <c r="J58" s="39"/>
-      <c r="K58" s="30"/>
-      <c r="L58" s="30"/>
-      <c r="M58" s="26"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="32"/>
     </row>
     <row r="59" spans="1:13" ht="32">
       <c r="A59" s="37"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="38"/>
-      <c r="F59" s="27"/>
+      <c r="F59" s="33"/>
       <c r="G59" s="15" t="s">
         <v>114</v>
       </c>
@@ -6441,17 +6468,17 @@
       </c>
       <c r="I59" s="18"/>
       <c r="J59" s="39"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="30"/>
-      <c r="M59" s="26"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="32"/>
     </row>
     <row r="60" spans="1:13" ht="32">
       <c r="A60" s="37"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
       <c r="E60" s="38"/>
-      <c r="F60" s="27"/>
+      <c r="F60" s="33"/>
       <c r="G60" s="15" t="s">
         <v>95</v>
       </c>
@@ -6460,42 +6487,42 @@
       </c>
       <c r="I60" s="18"/>
       <c r="J60" s="39"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="30"/>
-      <c r="M60" s="26"/>
+      <c r="K60" s="28"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="32"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="28"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="28"/>
-      <c r="K61" s="28"/>
-      <c r="L61" s="28"/>
-      <c r="M61" s="29"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="26"/>
+      <c r="M61" s="27"/>
     </row>
     <row r="62" spans="1:13" ht="16">
       <c r="A62" s="37">
         <v>10</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="D62" s="32" t="s">
         <v>122</v>
       </c>
       <c r="E62" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="F62" s="26" t="s">
+      <c r="F62" s="32" t="s">
         <v>117</v>
       </c>
       <c r="G62" s="15" t="s">
@@ -6508,21 +6535,21 @@
       <c r="J62" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K62" s="30" t="s">
+      <c r="K62" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L62" s="30" t="s">
+      <c r="L62" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="M62" s="26"/>
+      <c r="M62" s="32"/>
     </row>
     <row r="63" spans="1:13" ht="32">
       <c r="A63" s="37"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
       <c r="E63" s="38"/>
-      <c r="F63" s="27"/>
+      <c r="F63" s="33"/>
       <c r="G63" s="15" t="s">
         <v>81</v>
       </c>
@@ -6531,17 +6558,17 @@
       </c>
       <c r="I63" s="18"/>
       <c r="J63" s="39"/>
-      <c r="K63" s="30"/>
-      <c r="L63" s="30"/>
-      <c r="M63" s="26"/>
+      <c r="K63" s="28"/>
+      <c r="L63" s="28"/>
+      <c r="M63" s="32"/>
     </row>
     <row r="64" spans="1:13" ht="32">
       <c r="A64" s="37"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="26"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
       <c r="E64" s="38"/>
-      <c r="F64" s="27"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="15" t="s">
         <v>83</v>
       </c>
@@ -6550,17 +6577,17 @@
       </c>
       <c r="I64" s="18"/>
       <c r="J64" s="39"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="30"/>
-      <c r="M64" s="26"/>
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="M64" s="32"/>
     </row>
     <row r="65" spans="1:13" ht="112">
       <c r="A65" s="37"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
       <c r="E65" s="38"/>
-      <c r="F65" s="27"/>
+      <c r="F65" s="33"/>
       <c r="G65" s="15" t="s">
         <v>89</v>
       </c>
@@ -6569,17 +6596,17 @@
       </c>
       <c r="I65" s="18"/>
       <c r="J65" s="39"/>
-      <c r="K65" s="30"/>
-      <c r="L65" s="30"/>
-      <c r="M65" s="26"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="32"/>
     </row>
     <row r="66" spans="1:13" ht="32">
       <c r="A66" s="37"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
       <c r="E66" s="38"/>
-      <c r="F66" s="27"/>
+      <c r="F66" s="33"/>
       <c r="G66" s="15" t="s">
         <v>123</v>
       </c>
@@ -6588,17 +6615,17 @@
       </c>
       <c r="I66" s="18"/>
       <c r="J66" s="39"/>
-      <c r="K66" s="30"/>
-      <c r="L66" s="30"/>
-      <c r="M66" s="26"/>
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="32"/>
     </row>
     <row r="67" spans="1:13" ht="32">
       <c r="A67" s="37"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
       <c r="E67" s="38"/>
-      <c r="F67" s="27"/>
+      <c r="F67" s="33"/>
       <c r="G67" s="15" t="s">
         <v>94</v>
       </c>
@@ -6607,17 +6634,17 @@
       </c>
       <c r="I67" s="18"/>
       <c r="J67" s="39"/>
-      <c r="K67" s="30"/>
-      <c r="L67" s="30"/>
-      <c r="M67" s="26"/>
+      <c r="K67" s="28"/>
+      <c r="L67" s="28"/>
+      <c r="M67" s="32"/>
     </row>
     <row r="68" spans="1:13" ht="32">
       <c r="A68" s="37"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
+      <c r="B68" s="32"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
       <c r="E68" s="38"/>
-      <c r="F68" s="27"/>
+      <c r="F68" s="33"/>
       <c r="G68" s="15" t="s">
         <v>95</v>
       </c>
@@ -6626,36 +6653,36 @@
       </c>
       <c r="I68" s="18"/>
       <c r="J68" s="39"/>
-      <c r="K68" s="30"/>
-      <c r="L68" s="30"/>
-      <c r="M68" s="26"/>
+      <c r="K68" s="28"/>
+      <c r="L68" s="28"/>
+      <c r="M68" s="32"/>
     </row>
     <row r="69" spans="1:13">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="29"/>
+      <c r="A69" s="26"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="26"/>
+      <c r="K69" s="26"/>
+      <c r="L69" s="26"/>
+      <c r="M69" s="27"/>
     </row>
     <row r="70" spans="1:13" ht="16" customHeight="1">
       <c r="A70" s="37">
         <v>11</v>
       </c>
-      <c r="B70" s="26" t="s">
+      <c r="B70" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="C70" s="26" t="s">
+      <c r="C70" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="D70" s="26" t="s">
+      <c r="D70" s="32" t="s">
         <v>127</v>
       </c>
       <c r="E70" s="38" t="s">
@@ -6674,19 +6701,19 @@
       <c r="J70" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K70" s="30" t="s">
+      <c r="K70" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L70" s="30" t="s">
+      <c r="L70" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="M70" s="26"/>
+      <c r="M70" s="32"/>
     </row>
     <row r="71" spans="1:13" ht="32">
       <c r="A71" s="37"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
       <c r="E71" s="38"/>
       <c r="F71" s="35"/>
       <c r="G71" s="15" t="s">
@@ -6697,15 +6724,15 @@
       </c>
       <c r="I71" s="18"/>
       <c r="J71" s="39"/>
-      <c r="K71" s="30"/>
-      <c r="L71" s="30"/>
-      <c r="M71" s="26"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
+      <c r="M71" s="32"/>
     </row>
     <row r="72" spans="1:13" ht="64">
       <c r="A72" s="37"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
       <c r="E72" s="38"/>
       <c r="F72" s="35"/>
       <c r="G72" s="15" t="s">
@@ -6716,15 +6743,15 @@
       </c>
       <c r="I72" s="18"/>
       <c r="J72" s="39"/>
-      <c r="K72" s="30"/>
-      <c r="L72" s="30"/>
-      <c r="M72" s="26"/>
+      <c r="K72" s="28"/>
+      <c r="L72" s="28"/>
+      <c r="M72" s="32"/>
     </row>
     <row r="73" spans="1:13" ht="112">
       <c r="A73" s="37"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
       <c r="E73" s="38"/>
       <c r="F73" s="35"/>
       <c r="G73" s="15" t="s">
@@ -6735,15 +6762,15 @@
       </c>
       <c r="I73" s="18"/>
       <c r="J73" s="39"/>
-      <c r="K73" s="30"/>
-      <c r="L73" s="30"/>
-      <c r="M73" s="26"/>
+      <c r="K73" s="28"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="32"/>
     </row>
     <row r="74" spans="1:13" ht="32">
       <c r="A74" s="37"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
       <c r="E74" s="38"/>
       <c r="F74" s="35"/>
       <c r="G74" s="15" t="s">
@@ -6754,15 +6781,15 @@
       </c>
       <c r="I74" s="18"/>
       <c r="J74" s="39"/>
-      <c r="K74" s="30"/>
-      <c r="L74" s="30"/>
-      <c r="M74" s="26"/>
+      <c r="K74" s="28"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="32"/>
     </row>
     <row r="75" spans="1:13" ht="32">
       <c r="A75" s="37"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
       <c r="E75" s="38"/>
       <c r="F75" s="36"/>
       <c r="G75" s="15" t="s">
@@ -6773,42 +6800,42 @@
       </c>
       <c r="I75" s="18"/>
       <c r="J75" s="39"/>
-      <c r="K75" s="30"/>
-      <c r="L75" s="30"/>
-      <c r="M75" s="26"/>
+      <c r="K75" s="28"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="32"/>
     </row>
     <row r="76" spans="1:13">
-      <c r="A76" s="28"/>
-      <c r="B76" s="28"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="28"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="28"/>
-      <c r="K76" s="28"/>
-      <c r="L76" s="28"/>
-      <c r="M76" s="29"/>
+      <c r="A76" s="26"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
+      <c r="G76" s="26"/>
+      <c r="H76" s="26"/>
+      <c r="I76" s="26"/>
+      <c r="J76" s="26"/>
+      <c r="K76" s="26"/>
+      <c r="L76" s="26"/>
+      <c r="M76" s="27"/>
     </row>
     <row r="77" spans="1:13" ht="16">
       <c r="A77" s="37">
         <v>12</v>
       </c>
-      <c r="B77" s="26" t="s">
+      <c r="B77" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C77" s="26" t="s">
+      <c r="C77" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="D77" s="26" t="s">
+      <c r="D77" s="32" t="s">
         <v>137</v>
       </c>
       <c r="E77" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="F77" s="26" t="s">
+      <c r="F77" s="32" t="s">
         <v>135</v>
       </c>
       <c r="G77" s="15" t="s">
@@ -6821,21 +6848,21 @@
       <c r="J77" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K77" s="30" t="s">
+      <c r="K77" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L77" s="30" t="s">
+      <c r="L77" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="M77" s="26"/>
+      <c r="M77" s="32"/>
     </row>
     <row r="78" spans="1:13" ht="32">
       <c r="A78" s="37"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
       <c r="E78" s="38"/>
-      <c r="F78" s="27"/>
+      <c r="F78" s="33"/>
       <c r="G78" s="15" t="s">
         <v>81</v>
       </c>
@@ -6844,17 +6871,17 @@
       </c>
       <c r="I78" s="18"/>
       <c r="J78" s="39"/>
-      <c r="K78" s="30"/>
-      <c r="L78" s="30"/>
-      <c r="M78" s="26"/>
+      <c r="K78" s="28"/>
+      <c r="L78" s="28"/>
+      <c r="M78" s="32"/>
     </row>
     <row r="79" spans="1:13" ht="112">
       <c r="A79" s="37"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="26"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
       <c r="E79" s="38"/>
-      <c r="F79" s="27"/>
+      <c r="F79" s="33"/>
       <c r="G79" s="15" t="s">
         <v>52</v>
       </c>
@@ -6863,17 +6890,17 @@
       </c>
       <c r="I79" s="18"/>
       <c r="J79" s="39"/>
-      <c r="K79" s="30"/>
-      <c r="L79" s="30"/>
-      <c r="M79" s="26"/>
+      <c r="K79" s="28"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="32"/>
     </row>
     <row r="80" spans="1:13" ht="32">
       <c r="A80" s="37"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
       <c r="E80" s="38"/>
-      <c r="F80" s="27"/>
+      <c r="F80" s="33"/>
       <c r="G80" s="15" t="s">
         <v>55</v>
       </c>
@@ -6882,42 +6909,42 @@
       </c>
       <c r="I80" s="18"/>
       <c r="J80" s="39"/>
-      <c r="K80" s="30"/>
-      <c r="L80" s="30"/>
-      <c r="M80" s="26"/>
+      <c r="K80" s="28"/>
+      <c r="L80" s="28"/>
+      <c r="M80" s="32"/>
     </row>
     <row r="81" spans="1:13">
-      <c r="A81" s="28"/>
-      <c r="B81" s="28"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="28"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
-      <c r="K81" s="28"/>
-      <c r="L81" s="28"/>
-      <c r="M81" s="29"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="26"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="26"/>
+      <c r="L81" s="26"/>
+      <c r="M81" s="27"/>
     </row>
     <row r="82" spans="1:13" ht="16">
       <c r="A82" s="37">
         <v>13</v>
       </c>
-      <c r="B82" s="26" t="s">
+      <c r="B82" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C82" s="26" t="s">
+      <c r="C82" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="D82" s="26" t="s">
+      <c r="D82" s="32" t="s">
         <v>134</v>
       </c>
       <c r="E82" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="26" t="s">
+      <c r="F82" s="32" t="s">
         <v>118</v>
       </c>
       <c r="G82" s="15" t="s">
@@ -6930,21 +6957,21 @@
       <c r="J82" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="K82" s="30" t="s">
+      <c r="K82" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="L82" s="30" t="s">
+      <c r="L82" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="M82" s="26"/>
+      <c r="M82" s="32"/>
     </row>
     <row r="83" spans="1:13" ht="32">
       <c r="A83" s="37"/>
-      <c r="B83" s="26"/>
-      <c r="C83" s="26"/>
-      <c r="D83" s="26"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="32"/>
       <c r="E83" s="38"/>
-      <c r="F83" s="27"/>
+      <c r="F83" s="33"/>
       <c r="G83" s="15" t="s">
         <v>81</v>
       </c>
@@ -6953,17 +6980,17 @@
       </c>
       <c r="I83" s="18"/>
       <c r="J83" s="39"/>
-      <c r="K83" s="30"/>
-      <c r="L83" s="30"/>
-      <c r="M83" s="26"/>
+      <c r="K83" s="28"/>
+      <c r="L83" s="28"/>
+      <c r="M83" s="32"/>
     </row>
     <row r="84" spans="1:13" ht="112">
       <c r="A84" s="37"/>
-      <c r="B84" s="26"/>
-      <c r="C84" s="26"/>
-      <c r="D84" s="26"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
       <c r="E84" s="38"/>
-      <c r="F84" s="27"/>
+      <c r="F84" s="33"/>
       <c r="G84" s="15" t="s">
         <v>52</v>
       </c>
@@ -6972,17 +6999,17 @@
       </c>
       <c r="I84" s="18"/>
       <c r="J84" s="39"/>
-      <c r="K84" s="30"/>
-      <c r="L84" s="30"/>
-      <c r="M84" s="26"/>
+      <c r="K84" s="28"/>
+      <c r="L84" s="28"/>
+      <c r="M84" s="32"/>
     </row>
     <row r="85" spans="1:13" ht="32">
       <c r="A85" s="37"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="26"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
       <c r="E85" s="38"/>
-      <c r="F85" s="27"/>
+      <c r="F85" s="33"/>
       <c r="G85" s="15" t="s">
         <v>55</v>
       </c>
@@ -6991,24 +7018,24 @@
       </c>
       <c r="I85" s="18"/>
       <c r="J85" s="39"/>
-      <c r="K85" s="30"/>
-      <c r="L85" s="30"/>
-      <c r="M85" s="26"/>
+      <c r="K85" s="28"/>
+      <c r="L85" s="28"/>
+      <c r="M85" s="32"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="28"/>
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-      <c r="J86" s="28"/>
-      <c r="K86" s="28"/>
-      <c r="L86" s="28"/>
-      <c r="M86" s="29"/>
+      <c r="A86" s="26"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
+      <c r="J86" s="26"/>
+      <c r="K86" s="26"/>
+      <c r="L86" s="26"/>
+      <c r="M86" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="143">
@@ -7048,6 +7075,7 @@
     <mergeCell ref="K19:K22"/>
     <mergeCell ref="M19:M22"/>
     <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F24:F27"/>
     <mergeCell ref="A33:M33"/>
     <mergeCell ref="A28:M28"/>
     <mergeCell ref="A29:A32"/>
@@ -7058,6 +7086,7 @@
     <mergeCell ref="J29:J32"/>
     <mergeCell ref="K29:K32"/>
     <mergeCell ref="M29:M32"/>
+    <mergeCell ref="F29:F32"/>
     <mergeCell ref="A38:M38"/>
     <mergeCell ref="J34:J37"/>
     <mergeCell ref="K34:K37"/>
@@ -7067,6 +7096,7 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="E34:E37"/>
+    <mergeCell ref="F34:F37"/>
     <mergeCell ref="A46:M46"/>
     <mergeCell ref="J39:J45"/>
     <mergeCell ref="K39:K45"/>
@@ -7076,6 +7106,7 @@
     <mergeCell ref="C39:C45"/>
     <mergeCell ref="D39:D45"/>
     <mergeCell ref="E39:E45"/>
+    <mergeCell ref="F39:F45"/>
     <mergeCell ref="A53:M53"/>
     <mergeCell ref="A47:A52"/>
     <mergeCell ref="B47:B52"/>
@@ -7085,6 +7116,7 @@
     <mergeCell ref="J47:J52"/>
     <mergeCell ref="K47:K52"/>
     <mergeCell ref="M47:M52"/>
+    <mergeCell ref="F47:F52"/>
     <mergeCell ref="A54:A60"/>
     <mergeCell ref="B54:B60"/>
     <mergeCell ref="C54:C60"/>
@@ -7114,11 +7146,6 @@
     <mergeCell ref="K70:K75"/>
     <mergeCell ref="M70:M75"/>
     <mergeCell ref="F70:F75"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D85"/>
-    <mergeCell ref="E82:E85"/>
-    <mergeCell ref="J82:J85"/>
-    <mergeCell ref="K82:K85"/>
     <mergeCell ref="M82:M85"/>
     <mergeCell ref="F82:F85"/>
     <mergeCell ref="A76:M76"/>
@@ -7131,11 +7158,6 @@
     <mergeCell ref="K77:K80"/>
     <mergeCell ref="M77:M80"/>
     <mergeCell ref="F77:F80"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="F39:F45"/>
-    <mergeCell ref="F47:F52"/>
     <mergeCell ref="A86:M86"/>
     <mergeCell ref="L9:L12"/>
     <mergeCell ref="L14:L17"/>
@@ -7155,6 +7177,11 @@
     <mergeCell ref="A81:M81"/>
     <mergeCell ref="A82:A85"/>
     <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D85"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="J82:J85"/>
+    <mergeCell ref="K82:K85"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:E9 G9:G12 H11 H16 G14:G17 G50:G52 H50:H51 G78 G80 H21 G36:G37 G26:G27 H26 G31:G32 G42:G45 H42 G67:G68 G57 H57:H59 G59:G60 G70:G72 H72:H74 G74:G75 G85">
     <cfRule type="expression" dxfId="365" priority="579">

</xml_diff>